<commit_message>
new formats for the hiatus
</commit_message>
<xml_diff>
--- a/ui/components/cavaillon_sharedlinks.xlsx
+++ b/ui/components/cavaillon_sharedlinks.xlsx
@@ -497,7 +497,11 @@
           <t>Service providers performance</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>hiatus</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>HANWASH USER</t>
@@ -505,7 +509,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Service providers performance: </t>
+          <t>Service providers performance: hiatus</t>
         </is>
       </c>
     </row>
@@ -515,7 +519,11 @@
           <t>Investment status</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>hiatus</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>HANWASH USER</t>
@@ -523,7 +531,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Investment status: </t>
+          <t>Investment status: hiatus</t>
         </is>
       </c>
     </row>
@@ -533,7 +541,11 @@
           <t>Lessons Learned</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>hiatus</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>HANWASH USER</t>
@@ -541,7 +553,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Lessons Learned: </t>
+          <t>Lessons Learned: hiatus</t>
         </is>
       </c>
     </row>

</xml_diff>